<commit_message>
Last changes in the project
</commit_message>
<xml_diff>
--- a/documents/StandarizedVariableAnalysis.xlsx
+++ b/documents/StandarizedVariableAnalysis.xlsx
@@ -16,7 +16,6 @@
     <sheet name="PCA" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1278,11 +1277,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438670888"/>
-        <c:axId val="438663440"/>
+        <c:axId val="389213776"/>
+        <c:axId val="389214168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="438670888"/>
+        <c:axId val="389213776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438663440"/>
+        <c:crossAx val="389214168"/>
         <c:crossesAt val="-1.5"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1332,7 +1331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="438663440"/>
+        <c:axId val="389214168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,6 +1372,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1433,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438670888"/>
+        <c:crossAx val="389213776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2112,11 +2112,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438621976"/>
-        <c:axId val="438620016"/>
+        <c:axId val="466833392"/>
+        <c:axId val="466832216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="438621976"/>
+        <c:axId val="466833392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438620016"/>
+        <c:crossAx val="466832216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2166,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="438620016"/>
+        <c:axId val="466832216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +2247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438621976"/>
+        <c:crossAx val="466833392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2596,11 +2596,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438621192"/>
-        <c:axId val="438622368"/>
+        <c:axId val="466834568"/>
+        <c:axId val="466834960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="438621192"/>
+        <c:axId val="466834568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2643,7 +2643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438622368"/>
+        <c:crossAx val="466834960"/>
         <c:crossesAt val="-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2651,7 +2651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="438622368"/>
+        <c:axId val="466834960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,7 +2752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438621192"/>
+        <c:crossAx val="466834568"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3099,11 +3099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438617272"/>
-        <c:axId val="438618056"/>
+        <c:axId val="466835744"/>
+        <c:axId val="388980744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="438617272"/>
+        <c:axId val="466835744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3145,7 +3145,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438618056"/>
+        <c:crossAx val="388980744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3153,7 +3153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="438618056"/>
+        <c:axId val="388980744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,7 +3234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438617272"/>
+        <c:crossAx val="466835744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3329,6 +3329,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4328,11 +4329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="284142672"/>
-        <c:axId val="284723776"/>
+        <c:axId val="388985056"/>
+        <c:axId val="388985840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="284142672"/>
+        <c:axId val="388985056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4389,12 +4390,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284723776"/>
+        <c:crossAx val="388985840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284723776"/>
+        <c:axId val="388985840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4451,7 +4452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284142672"/>
+        <c:crossAx val="388985056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4515,6 +4516,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4674,11 +4676,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="284726128"/>
-        <c:axId val="284722992"/>
+        <c:axId val="322181128"/>
+        <c:axId val="322185048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="284726128"/>
+        <c:axId val="322181128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4735,12 +4737,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284722992"/>
+        <c:crossAx val="322185048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284722992"/>
+        <c:axId val="322185048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4797,7 +4799,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284726128"/>
+        <c:crossAx val="322181128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4861,6 +4863,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5860,11 +5863,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="284724952"/>
-        <c:axId val="284725344"/>
+        <c:axId val="322188184"/>
+        <c:axId val="322182696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="284724952"/>
+        <c:axId val="322188184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5921,12 +5924,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284725344"/>
+        <c:crossAx val="322182696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284725344"/>
+        <c:axId val="322182696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5983,7 +5986,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284724952"/>
+        <c:crossAx val="322188184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6221,11 +6224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438667752"/>
-        <c:axId val="438665008"/>
+        <c:axId val="389211816"/>
+        <c:axId val="389216128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="438667752"/>
+        <c:axId val="389211816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6267,7 +6270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438665008"/>
+        <c:crossAx val="389216128"/>
         <c:crossesAt val="-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6275,7 +6278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="438665008"/>
+        <c:axId val="389216128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6316,6 +6319,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6376,7 +6380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438667752"/>
+        <c:crossAx val="389211816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6655,11 +6659,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375507856"/>
-        <c:axId val="375510992"/>
+        <c:axId val="389212992"/>
+        <c:axId val="389213384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375507856"/>
+        <c:axId val="389212992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6701,7 +6705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375510992"/>
+        <c:crossAx val="389213384"/>
         <c:crossesAt val="-3"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6709,7 +6713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375510992"/>
+        <c:axId val="389213384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6810,7 +6814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375507856"/>
+        <c:crossAx val="389212992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7089,11 +7093,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="375505112"/>
-        <c:axId val="375505504"/>
+        <c:axId val="389215344"/>
+        <c:axId val="389215736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="375505112"/>
+        <c:axId val="389215344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7135,7 +7139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375505504"/>
+        <c:crossAx val="389215736"/>
         <c:crossesAt val="-3"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7143,7 +7147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="375505504"/>
+        <c:axId val="389215736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7244,7 +7248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="375505112"/>
+        <c:crossAx val="389215344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7523,11 +7527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="284139536"/>
-        <c:axId val="284141496"/>
+        <c:axId val="388986232"/>
+        <c:axId val="388983880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="284139536"/>
+        <c:axId val="388986232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7569,7 +7573,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284141496"/>
+        <c:crossAx val="388983880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7577,7 +7581,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="284141496"/>
+        <c:axId val="388983880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7683,7 +7687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284139536"/>
+        <c:crossAx val="388986232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7913,11 +7917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="376648928"/>
-        <c:axId val="438617664"/>
+        <c:axId val="466836528"/>
+        <c:axId val="466830648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="376648928"/>
+        <c:axId val="466836528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7985,6 +7989,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8051,12 +8056,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438617664"/>
+        <c:crossAx val="466830648"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438617664"/>
+        <c:axId val="466830648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8116,6 +8121,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8182,7 +8188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376648928"/>
+        <c:crossAx val="466836528"/>
         <c:crossesAt val="-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8422,11 +8428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438622760"/>
-        <c:axId val="438623152"/>
+        <c:axId val="466834176"/>
+        <c:axId val="466832608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438622760"/>
+        <c:axId val="466834176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8486,6 +8492,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8552,12 +8559,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438623152"/>
+        <c:crossAx val="466832608"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438623152"/>
+        <c:axId val="466832608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8622,6 +8629,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8688,7 +8696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438622760"/>
+        <c:crossAx val="466834176"/>
         <c:crossesAt val="-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8702,6 +8710,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8918,11 +8927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438620800"/>
-        <c:axId val="438619232"/>
+        <c:axId val="466836136"/>
+        <c:axId val="466833000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438620800"/>
+        <c:axId val="466836136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9023,12 +9032,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438619232"/>
+        <c:crossAx val="466833000"/>
         <c:crossesAt val="-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438619232"/>
+        <c:axId val="466833000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9129,7 +9138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438620800"/>
+        <c:crossAx val="466836136"/>
         <c:crossesAt val="-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9389,11 +9398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438618448"/>
-        <c:axId val="438623936"/>
+        <c:axId val="466831432"/>
+        <c:axId val="466829864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438618448"/>
+        <c:axId val="466831432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9494,12 +9503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438623936"/>
+        <c:crossAx val="466829864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438623936"/>
+        <c:axId val="466829864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9600,7 +9609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438618448"/>
+        <c:crossAx val="466831432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26563,8 +26572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AG154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:AG12"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -48843,7 +48852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A52" sqref="A52:A56"/>
     </sheetView>
   </sheetViews>

</xml_diff>